<commit_message>
v2 portfolio with project
</commit_message>
<xml_diff>
--- a/docs/PAUL-Thomas-Synthèse-Epreuve-E5-2025.xlsx
+++ b/docs/PAUL-Thomas-Synthèse-Epreuve-E5-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\portfolio\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5DF7FAC-39E1-4ECE-8A6C-7F8E5602C794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D85B91-920E-45C1-BA7E-BA028DD1C4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -156,21 +155,33 @@
     <t>Centre de formation : ORT MONTREUIL DANIEL MAYER</t>
   </si>
   <si>
-    <t xml:space="preserve">Projet Veliko : reproduction de l'application Velib avec des fonctionnalitées supplémentaires (Php,  Java, mysql)
-</t>
-  </si>
-  <si>
     <t>10/09/2024 - 24/03/2025</t>
   </si>
   <si>
     <t>Creation d'un inventaire du materiel informatique reseau au cœur d'air-France</t>
-  </si>
-  <si>
-    <t>20/05/2024 - 2/07/2024</t>
   </si>
   <si>
     <t xml:space="preserve">PortFolio : création d'un portfolio (php)
 </t>
+  </si>
+  <si>
+    <t>02/09/2024 - 16/11/2024</t>
+  </si>
+  <si>
+    <t>20/05/2024 - 02/07/2024</t>
+  </si>
+  <si>
+    <t>GLPI : Gestionnaire Libre de Parc Informatique</t>
+  </si>
+  <si>
+    <t>Projet Veliko Web : reproduction de l'application Velib avec des fonctionnalitées supplémentaires (Php,  Java, mysql)</t>
+  </si>
+  <si>
+    <t>Projet Veliko Java : Gestion des utilisateurs, Gestion du parc ⇒ MAP,
+Dashboard ⇒ Statistiques</t>
+  </si>
+  <si>
+    <t>24/03/2024 - 22/12/2024</t>
   </si>
 </sst>
 </file>
@@ -180,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -242,12 +253,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -660,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -698,110 +703,124 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -819,6 +838,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1113,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="32" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1127,84 +1163,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" cm="1">
+      <c r="A6" s="33" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">A6:H13+K7</f>
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1227,24 +1263,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1284,16 +1320,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1332,17 +1368,17 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="B9" s="47">
+        <v>2023</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="14"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1381,14 +1417,17 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="23"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1426,14 +1465,18 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+      <c r="A11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="14"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1471,14 +1514,18 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="14"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1518,12 +1565,12 @@
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1563,12 +1610,12 @@
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1608,12 +1655,12 @@
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1653,12 +1700,12 @@
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1698,12 +1745,12 @@
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1743,12 +1790,12 @@
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1786,16 +1833,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1834,17 +1881,17 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1882,14 +1929,13 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="8"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1929,12 +1975,12 @@
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1973,13 +2019,12 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2019,12 +2064,12 @@
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2064,12 +2109,12 @@
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2109,12 +2154,12 @@
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2152,16 +2197,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2201,12 +2246,12 @@
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2246,12 +2291,12 @@
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2291,12 +2336,12 @@
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2336,12 +2381,12 @@
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2381,12 +2426,12 @@
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="14"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2426,12 +2471,12 @@
     <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="14"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2471,12 +2516,12 @@
     <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2606,11 +2651,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2618,6 +2658,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2628,23 +2673,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="21cc5093-9163-4e27-a3aa-cc0a4152508a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030A3E2461DF3DE4A944E427B9A96A21D" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f21990113fb28ea316886c90014d687c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21cc5093-9163-4e27-a3aa-cc0a4152508a" xmlns:ns4="978d5f1d-33bb-45b4-be03-11c1668f1fd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edf4a97f6ff384928791003657ad5938" ns3:_="" ns4:_="">
     <xsd:import namespace="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
@@ -2871,32 +2899,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7BE212-4AE1-46DA-9E63-16F5B02F1458}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="978d5f1d-33bb-45b4-be03-11c1668f1fd8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{135C126B-569F-407D-9EC3-0F302F205D36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="21cc5093-9163-4e27-a3aa-cc0a4152508a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20699FD3-F535-4112-B89C-C94FE56D5134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2913,4 +2933,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{135C126B-569F-407D-9EC3-0F302F205D36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7BE212-4AE1-46DA-9E63-16F5B02F1458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="978d5f1d-33bb-45b4-be03-11c1668f1fd8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
edit tableau de synthèse
</commit_message>
<xml_diff>
--- a/docs/PAUL-Thomas-Synthèse-Epreuve-E5-2025.xlsx
+++ b/docs/PAUL-Thomas-Synthèse-Epreuve-E5-2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\portfolio\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D85B91-920E-45C1-BA7E-BA028DD1C4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC79B7A7-CA96-4489-9639-23AD0D1FD73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -168,9 +168,6 @@
     <t>02/09/2024 - 16/11/2024</t>
   </si>
   <si>
-    <t>20/05/2024 - 02/07/2024</t>
-  </si>
-  <si>
     <t>GLPI : Gestionnaire Libre de Parc Informatique</t>
   </si>
   <si>
@@ -182,6 +179,15 @@
   </si>
   <si>
     <t>24/03/2024 - 22/12/2024</t>
+  </si>
+  <si>
+    <t>Retranscription de test d'integration de TypeScript en Kotlin au cœur de Biron Data</t>
+  </si>
+  <si>
+    <t>06/01/2025 - 07/02/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  20/05/2024 - 02/07/2024</t>
   </si>
 </sst>
 </file>
@@ -736,72 +742,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <extLst>
@@ -821,6 +761,72 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1149,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="50" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1163,60 +1169,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="50"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="24" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="17" t="s">
@@ -1224,23 +1230,23 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" cm="1">
+      <c r="A6" s="29" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">A6:H13+K7</f>
         <v>0</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1263,8 +1269,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
@@ -1320,16 +1326,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1368,9 +1374,9 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="47">
+        <v>30</v>
+      </c>
+      <c r="B9" s="25">
         <v>2023</v>
       </c>
       <c r="C9" s="19"/>
@@ -1419,7 +1425,7 @@
       <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="13"/>
@@ -1466,9 +1472,9 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="22"/>
@@ -1515,10 +1521,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>34</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1833,16 +1839,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1884,7 +1890,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="20"/>
@@ -2197,16 +2203,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2244,14 +2250,18 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="23"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2651,6 +2661,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2658,11 +2673,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2673,6 +2683,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="21cc5093-9163-4e27-a3aa-cc0a4152508a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030A3E2461DF3DE4A944E427B9A96A21D" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f21990113fb28ea316886c90014d687c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21cc5093-9163-4e27-a3aa-cc0a4152508a" xmlns:ns4="978d5f1d-33bb-45b4-be03-11c1668f1fd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edf4a97f6ff384928791003657ad5938" ns3:_="" ns4:_="">
     <xsd:import namespace="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
@@ -2899,24 +2926,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7BE212-4AE1-46DA-9E63-16F5B02F1458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="978d5f1d-33bb-45b4-be03-11c1668f1fd8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="21cc5093-9163-4e27-a3aa-cc0a4152508a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{135C126B-569F-407D-9EC3-0F302F205D36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20699FD3-F535-4112-B89C-C94FE56D5134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2933,29 +2968,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{135C126B-569F-407D-9EC3-0F302F205D36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7BE212-4AE1-46DA-9E63-16F5B02F1458}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="978d5f1d-33bb-45b4-be03-11c1668f1fd8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="21cc5093-9163-4e27-a3aa-cc0a4152508a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>